<commit_message>
SSDM-10984 : Vocabulary Code -> Vocabulary code header to follow same casing pattern as other headers
</commit_message>
<xml_diff>
--- a/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/general_eln_settings.xlsx
+++ b/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/general_eln_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariapukhliakova/git/openbis/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanf/Documents/sissource/openbis/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDCD605-E3FD-1146-AAE6-E81CD467FB4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D8D4B-FF83-E24C-B6A7-C010552A1F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="1300" windowWidth="27240" windowHeight="16440" xr2:uid="{8C518BD6-93EE-234E-BC6F-85CE38D9A7C4}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>Data type</t>
   </si>
   <si>
-    <t>Vocabulary Code</t>
-  </si>
-  <si>
     <t>Dynamic script</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>General info</t>
+  </si>
+  <si>
+    <t>Vocabulary code</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:XFC31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,6 +604,7 @@
     <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="28.5" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="19" x14ac:dyDescent="0.25">
@@ -12960,13 +12961,13 @@
         <v>17</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
@@ -12974,7 +12975,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="9" t="b">
         <v>0</v>
@@ -12983,13 +12984,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="10" t="s">
@@ -13002,7 +13003,7 @@
     </row>
     <row r="7" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -13023,7 +13024,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -13049,17 +13050,17 @@
       <c r="G10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>18</v>
+      <c r="H10" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>2</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
@@ -13067,7 +13068,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>0</v>
@@ -13076,16 +13077,16 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="17" x14ac:dyDescent="0.2">
@@ -13112,7 +13113,7 @@
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2"/>
     </row>
@@ -13130,10 +13131,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -13142,20 +13143,20 @@
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -13165,21 +13166,21 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13202,7 +13203,7 @@
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
SSDM-10984 : Refactoring and strict validation of headers, ongoing work
</commit_message>
<xml_diff>
--- a/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/general_eln_settings.xlsx
+++ b/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/general_eln_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanf/Documents/sissource/openbis/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D8D4B-FF83-E24C-B6A7-C010552A1F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DF1123-627E-1E49-B84F-66BAD1A1BBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1300" windowWidth="27240" windowHeight="16440" xr2:uid="{8C518BD6-93EE-234E-BC6F-85CE38D9A7C4}"/>
+    <workbookView xWindow="12360" yWindow="3620" windowWidth="27240" windowHeight="16440" xr2:uid="{8C518BD6-93EE-234E-BC6F-85CE38D9A7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="TYPES" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>SPACE</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Vocabulary code</t>
+  </si>
+  <si>
+    <t>Generated code prefix</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
   <dimension ref="A1:XFC31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,14 +631,18 @@
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="14" t="s">
+        <v>38</v>
+      </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -12927,10 +12934,9 @@
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="b">
+      <c r="D3" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -13015,7 +13021,10 @@
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>